<commit_message>
- move Utils to utils package
</commit_message>
<xml_diff>
--- a/src/test/resources/test-logger.xlsx
+++ b/src/test/resources/test-logger.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="15">
   <si>
     <t>ID</t>
   </si>
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -605,6 +605,34 @@
         <v>6</v>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -612,7 +640,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -720,6 +748,34 @@
         <v>8</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -727,7 +783,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -835,6 +891,34 @@
         <v>10</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -842,7 +926,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -950,6 +1034,34 @@
         <v>12</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -957,7 +1069,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1065,6 +1177,34 @@
         <v>14</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
- add TableTest and TableManagerTest
</commit_message>
<xml_diff>
--- a/src/test/resources/test-logger.xlsx
+++ b/src/test/resources/test-logger.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="15">
   <si>
     <t>ID</t>
   </si>
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -633,6 +633,48 @@
         <v>6</v>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -640,7 +682,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -776,6 +818,48 @@
         <v>8</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -783,7 +867,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -919,6 +1003,48 @@
         <v>10</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -926,7 +1052,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1062,6 +1188,48 @@
         <v>12</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -1069,7 +1237,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1205,6 +1373,48 @@
         <v>14</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>